<commit_message>
Adicionando melhorias no código Python para análise de dados
Neste commit, fizemos algumas melhorias no código Python para análise de dados. Agora, o código consulta tanto para PF como para PJ as regiões presentes nos dados e gera informações detalhadas para cada região na mesma aba da planilha para PF e PJ. Isso torna o relatório mais analítico, permitindo que tenhamos visibilidade dos números de cada região para ambas as pessoas físicas e pessoas jurídicas.

Essas melhorias tornam o código mais útil e eficiente, oferecendo insights adicionais sobre os dados de beneficiários ativos, valor da receita e valor das despesas. Essa atualização será incluída no meu portfólio no GitHub e ficará disponível para futuros projetos e análises de dados.
</commit_message>
<xml_diff>
--- a/analitica.xlsx
+++ b/analitica.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053F0726-C0F2-4AA6-87F8-1D5843869385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5D2D78-0368-4926-8860-A6B4D2F70267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="830" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8730" yWindow="4020" windowWidth="23805" windowHeight="11385" tabRatio="830" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Janeiro-ANALITICO 2023" sheetId="35" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3281" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3281" uniqueCount="58">
   <si>
     <t>PLANO</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>EU MEU NOME</t>
+  </si>
+  <si>
+    <t>Embu</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Osasco</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
   </si>
 </sst>
 </file>
@@ -567,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D69" sqref="D2:D69"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +832,7 @@
         <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M5">
         <v>3437</v>
@@ -873,7 +885,7 @@
         <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M6">
         <v>3438</v>
@@ -923,7 +935,7 @@
         <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M7">
         <v>3439</v>
@@ -973,7 +985,7 @@
         <v>20</v>
       </c>
       <c r="L8" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M8">
         <v>3440</v>
@@ -1023,7 +1035,7 @@
         <v>20</v>
       </c>
       <c r="L9" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M9">
         <v>3441</v>
@@ -1073,7 +1085,7 @@
         <v>20</v>
       </c>
       <c r="L10" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M10">
         <v>3442</v>
@@ -1123,7 +1135,7 @@
         <v>20</v>
       </c>
       <c r="L11" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M11">
         <v>3443</v>
@@ -1173,7 +1185,7 @@
         <v>20</v>
       </c>
       <c r="L12" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M12">
         <v>3444</v>
@@ -1223,7 +1235,7 @@
         <v>20</v>
       </c>
       <c r="L13" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M13">
         <v>3445</v>
@@ -1273,7 +1285,7 @@
         <v>20</v>
       </c>
       <c r="L14" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M14">
         <v>3446</v>
@@ -1323,7 +1335,7 @@
         <v>20</v>
       </c>
       <c r="L15" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M15">
         <v>3447</v>
@@ -1373,7 +1385,7 @@
         <v>20</v>
       </c>
       <c r="L16" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M16">
         <v>3448</v>
@@ -1423,7 +1435,7 @@
         <v>20</v>
       </c>
       <c r="L17" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M17">
         <v>3449</v>
@@ -1476,7 +1488,7 @@
         <v>20</v>
       </c>
       <c r="L18" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M18">
         <v>3450</v>
@@ -1526,7 +1538,7 @@
         <v>20</v>
       </c>
       <c r="L19" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M19">
         <v>3451</v>
@@ -1576,7 +1588,7 @@
         <v>20</v>
       </c>
       <c r="L20" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M20">
         <v>3452</v>
@@ -1626,7 +1638,7 @@
         <v>20</v>
       </c>
       <c r="L21" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M21">
         <v>3453</v>
@@ -1676,7 +1688,7 @@
         <v>20</v>
       </c>
       <c r="L22" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M22">
         <v>3454</v>
@@ -1726,7 +1738,7 @@
         <v>20</v>
       </c>
       <c r="L23" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M23">
         <v>3455</v>
@@ -4071,8 +4083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D67"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34:L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5781,7 +5793,7 @@
         <v>20</v>
       </c>
       <c r="L34" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M34">
         <v>3466</v>
@@ -5831,7 +5843,7 @@
         <v>20</v>
       </c>
       <c r="L35" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M35">
         <v>3467</v>
@@ -5881,7 +5893,7 @@
         <v>20</v>
       </c>
       <c r="L36" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M36">
         <v>3468</v>
@@ -5931,7 +5943,7 @@
         <v>20</v>
       </c>
       <c r="L37" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M37">
         <v>3469</v>
@@ -5981,7 +5993,7 @@
         <v>20</v>
       </c>
       <c r="L38" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M38">
         <v>3470</v>
@@ -6031,7 +6043,7 @@
         <v>20</v>
       </c>
       <c r="L39" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M39">
         <v>3471</v>
@@ -6081,7 +6093,7 @@
         <v>20</v>
       </c>
       <c r="L40" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M40">
         <v>3472</v>
@@ -6131,7 +6143,7 @@
         <v>20</v>
       </c>
       <c r="L41" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M41">
         <v>3473</v>
@@ -6181,7 +6193,7 @@
         <v>20</v>
       </c>
       <c r="L42" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M42">
         <v>3474</v>
@@ -6234,7 +6246,7 @@
         <v>20</v>
       </c>
       <c r="L43" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M43">
         <v>3475</v>
@@ -6284,7 +6296,7 @@
         <v>20</v>
       </c>
       <c r="L44" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M44">
         <v>3476</v>
@@ -6334,7 +6346,7 @@
         <v>20</v>
       </c>
       <c r="L45" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M45">
         <v>3477</v>
@@ -6384,7 +6396,7 @@
         <v>20</v>
       </c>
       <c r="L46" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M46">
         <v>3478</v>
@@ -6434,7 +6446,7 @@
         <v>20</v>
       </c>
       <c r="L47" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M47">
         <v>3479</v>
@@ -6484,7 +6496,7 @@
         <v>20</v>
       </c>
       <c r="L48" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M48">
         <v>3480</v>
@@ -6534,7 +6546,7 @@
         <v>20</v>
       </c>
       <c r="L49" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M49">
         <v>3481</v>
@@ -6584,7 +6596,7 @@
         <v>20</v>
       </c>
       <c r="L50" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M50">
         <v>3482</v>
@@ -6634,7 +6646,7 @@
         <v>20</v>
       </c>
       <c r="L51" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M51">
         <v>3483</v>
@@ -6684,7 +6696,7 @@
         <v>20</v>
       </c>
       <c r="L52" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M52">
         <v>3484</v>
@@ -6734,7 +6746,7 @@
         <v>20</v>
       </c>
       <c r="L53" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M53">
         <v>3485</v>
@@ -6784,7 +6796,7 @@
         <v>20</v>
       </c>
       <c r="L54" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M54">
         <v>3486</v>
@@ -6837,7 +6849,7 @@
         <v>20</v>
       </c>
       <c r="L55" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="M55">
         <v>3487</v>
@@ -7474,8 +7486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D65"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35:L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9233,7 +9245,7 @@
         <v>20</v>
       </c>
       <c r="L35" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="M35">
         <v>3467</v>
@@ -9283,7 +9295,7 @@
         <v>20</v>
       </c>
       <c r="L36" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="M36">
         <v>3468</v>
@@ -9333,7 +9345,7 @@
         <v>20</v>
       </c>
       <c r="L37" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="M37">
         <v>3469</v>
@@ -9383,7 +9395,7 @@
         <v>20</v>
       </c>
       <c r="L38" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="M38">
         <v>3470</v>
@@ -9433,7 +9445,7 @@
         <v>20</v>
       </c>
       <c r="L39" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="M39">
         <v>3471</v>
@@ -9483,7 +9495,7 @@
         <v>20</v>
       </c>
       <c r="L40" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="M40">
         <v>3472</v>
@@ -9533,7 +9545,7 @@
         <v>20</v>
       </c>
       <c r="L41" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="M41">
         <v>3473</v>
@@ -9583,7 +9595,7 @@
         <v>20</v>
       </c>
       <c r="L42" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="M42">
         <v>3474</v>
@@ -9636,7 +9648,7 @@
         <v>20</v>
       </c>
       <c r="L43" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="M43">
         <v>3475</v>
@@ -9686,7 +9698,7 @@
         <v>20</v>
       </c>
       <c r="L44" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="M44">
         <v>3476</v>
@@ -17453,8 +17465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q1429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17755,7 +17767,7 @@
         <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M6">
         <v>3438</v>
@@ -17805,7 +17817,7 @@
         <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M7">
         <v>3439</v>
@@ -17855,7 +17867,7 @@
         <v>20</v>
       </c>
       <c r="L8" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M8">
         <v>3440</v>
@@ -17905,7 +17917,7 @@
         <v>20</v>
       </c>
       <c r="L9" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M9">
         <v>3441</v>
@@ -17955,7 +17967,7 @@
         <v>20</v>
       </c>
       <c r="L10" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M10">
         <v>3442</v>
@@ -18005,7 +18017,7 @@
         <v>20</v>
       </c>
       <c r="L11" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M11">
         <v>3443</v>
@@ -18055,7 +18067,7 @@
         <v>20</v>
       </c>
       <c r="L12" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M12">
         <v>3444</v>
@@ -18105,7 +18117,7 @@
         <v>20</v>
       </c>
       <c r="L13" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M13">
         <v>3445</v>
@@ -18155,7 +18167,7 @@
         <v>20</v>
       </c>
       <c r="L14" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M14">
         <v>3446</v>
@@ -18205,7 +18217,7 @@
         <v>20</v>
       </c>
       <c r="L15" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M15">
         <v>3447</v>
@@ -18255,7 +18267,7 @@
         <v>20</v>
       </c>
       <c r="L16" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M16">
         <v>3448</v>
@@ -18305,7 +18317,7 @@
         <v>20</v>
       </c>
       <c r="L17" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M17">
         <v>3449</v>
@@ -18358,7 +18370,7 @@
         <v>20</v>
       </c>
       <c r="L18" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M18">
         <v>3450</v>
@@ -18408,7 +18420,7 @@
         <v>20</v>
       </c>
       <c r="L19" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M19">
         <v>3451</v>
@@ -18458,7 +18470,7 @@
         <v>20</v>
       </c>
       <c r="L20" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M20">
         <v>3452</v>
@@ -18508,7 +18520,7 @@
         <v>20</v>
       </c>
       <c r="L21" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="M21">
         <v>3453</v>

</xml_diff>